<commit_message>
cross validation on Supervised ( to finish)  + NEW SCHEDULE
</commit_message>
<xml_diff>
--- a/SCHEDULE.xlsx
+++ b/SCHEDULE.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ettoremariotti/Desktop/Semmestre/BCI/Project/BCI-ThoughtRecognition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteociprian/OneDrive - Università degli Studi di Padova/università/magistrale/SecondoSemestre_Secondo_Anno/BCI/BCI-ThoughtRecognition/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Work Division" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">PRE PROCESSING </t>
   </si>
@@ -49,12 +49,6 @@
     <t>MATTEO</t>
   </si>
   <si>
-    <t>basic classification model</t>
-  </si>
-  <si>
-    <t>dataset augmentation </t>
-  </si>
-  <si>
     <t>ETTORE</t>
   </si>
   <si>
@@ -127,9 +121,6 @@
     <t>Dimensionality Reduction of channels</t>
   </si>
   <si>
-    <t>Deep Learning? (NN, RNN, CNN)</t>
-  </si>
-  <si>
     <t>The dataset is about one patient</t>
   </si>
   <si>
@@ -182,6 +173,21 @@
   </si>
   <si>
     <t>2 cell una per il YES, una per il NO</t>
+  </si>
+  <si>
+    <t>CNN</t>
+  </si>
+  <si>
+    <t>basic classification model -- completing cross-validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataset augmentation ( ARMA ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wavelet </t>
+  </si>
+  <si>
+    <t>Feature exploration : osservare lo spettro per individuare frequenze principali</t>
   </si>
 </sst>
 </file>
@@ -218,12 +224,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -238,14 +256,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -522,14 +542,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="2" max="2" width="74.6640625" customWidth="1"/>
     <col min="3" max="3" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -537,11 +557,11 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>35</v>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -549,7 +569,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -561,47 +581,57 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>6</v>
+      <c r="B7" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>7</v>
+      <c r="B8" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>31</v>
+      <c r="B13" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>32</v>
+      <c r="B14" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -613,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="194" zoomScaleNormal="194" zoomScalePageLayoutView="194" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A3" zoomScale="136" zoomScaleNormal="194" zoomScalePageLayoutView="194" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -625,15 +655,15 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -641,15 +671,15 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -660,7 +690,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -671,7 +701,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -680,12 +710,12 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -696,70 +726,70 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
+      <c r="A10" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>28</v>
+      <c r="A15" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
         <v>46</v>
-      </c>
-      <c r="C20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -783,42 +813,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
-        <v>44</v>
+      <c r="B1" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
         <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>